<commit_message>
update change request form
</commit_message>
<xml_diff>
--- a/SaT - OUT/SCM YGDChangeRequestForm.xlsx
+++ b/SaT - OUT/SCM YGDChangeRequestForm.xlsx
@@ -17,9 +17,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
-    <t>Created On : &lt;dd/mm/yy&gt;</t>
-  </si>
-  <si>
     <t>Identification</t>
   </si>
   <si>
@@ -114,13 +111,16 @@
   </si>
   <si>
     <t>Title :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created On : </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +163,13 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -276,65 +283,68 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,239 +643,251 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="14" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" style="14" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="1" width="41.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20" style="7" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" ht="34.5" customHeight="1">
+      <c r="A2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="16"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="1:3" ht="5.25" customHeight="1">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" ht="18" customHeight="1">
+      <c r="A11" s="13"/>
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" ht="18" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A12" s="13"/>
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+    </row>
+    <row r="15" spans="1:3" ht="6" customHeight="1">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:3" ht="40.5" customHeight="1">
+      <c r="A17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+    </row>
+    <row r="18" spans="1:3" ht="3.75" customHeight="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="1:3" ht="30.75" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" ht="30.75" customHeight="1">
-      <c r="A20" s="5" t="s">
+      <c r="C20" s="13"/>
+    </row>
+    <row r="21" spans="1:3" ht="30.75" customHeight="1">
+      <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" ht="30.75" customHeight="1">
-      <c r="A21" s="17" t="s">
+      <c r="B21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="C21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="17" t="s">
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" ht="5.25" customHeight="1">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="7" t="s">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+    </row>
+    <row r="26" spans="1:3" ht="33.75" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:3" ht="33.75" customHeight="1">
-      <c r="A26" s="5" t="s">
+      <c r="C26" s="13"/>
+    </row>
+    <row r="27" spans="1:3" ht="17.25" customHeight="1">
+      <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" ht="17.25" customHeight="1">
-      <c r="A27" s="6" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" ht="18" customHeight="1">
+      <c r="A28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:3" ht="18" customHeight="1">
-      <c r="A28" s="18" t="s">
+      <c r="B28" s="11"/>
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="1:3" ht="42.75" customHeight="1">
+      <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-    </row>
-    <row r="29" spans="1:3" ht="28.5" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="B29" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" ht="46.5" customHeight="1">
+      <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:3" ht="27" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="8"/>
+      <c r="B30" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="A28:C28"/>
@@ -875,20 +897,8 @@
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
-  <pageMargins left="1.1200000000000001" right="0.7" top="0.75" bottom="0.75" header="0.65" footer="0.3"/>
+  <pageMargins left="1.18" right="0.35" top="0.75" bottom="0.75" header="0.65" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>